<commit_message>
Add seeding performance metrics
</commit_message>
<xml_diff>
--- a/report/Data.xlsx
+++ b/report/Data.xlsx
@@ -1,25 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24527"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\spacepyro\Projects\GraphColoring\report\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jvale\Documents\UT\AdvancedAlgorithms\finalProject\report\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D4170C4-144E-4638-9652-798304179CF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17490" windowHeight="10695"/>
+    <workbookView xWindow="-38520" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Metropolis Seeding" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="66">
   <si>
     <t>Row</t>
   </si>
@@ -182,12 +195,48 @@
   <si>
     <t>AntCol Experiment 7</t>
   </si>
+  <si>
+    <t>UN Metropolis 8 Threads B[.95,1]</t>
+  </si>
+  <si>
+    <t>UN Metropolis 8 Cooperative Beta = [.95, 1]</t>
+  </si>
+  <si>
+    <t>UN Metropolis 8 Cooperative Beta = [.97, .99]</t>
+  </si>
+  <si>
+    <t>UN Metropolis 8 Cooperative Beta = [.98, .99]</t>
+  </si>
+  <si>
+    <t>RandomMetropolis 8 Threads B[.95,1]</t>
+  </si>
+  <si>
+    <t>RandomMetropolis 8 Cooperative Beta = [.95, 1]</t>
+  </si>
+  <si>
+    <t>Random Metropolis 8 Cooperative Beta = [.97, .99]</t>
+  </si>
+  <si>
+    <t>Random Metropolis 8 Cooperative Beta = [.98, .99]</t>
+  </si>
+  <si>
+    <t>Seeding</t>
+  </si>
+  <si>
+    <t>Simple</t>
+  </si>
+  <si>
+    <t>Random</t>
+  </si>
+  <si>
+    <t>Unassigned neighbor</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -202,6 +251,24 @@
       <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="&quot;Times New Roman&quot;"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="4">
@@ -224,7 +291,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -232,11 +299,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -247,6 +329,14 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -278,7 +368,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle name="Sheet1-style" pivot="0" count="3">
+    <tableStyle name="Sheet1-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="headerRow" dxfId="2"/>
       <tableStyleElement type="firstRowStripe" dxfId="1"/>
       <tableStyleElement type="secondRowStripe" dxfId="0"/>
@@ -296,7 +386,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
@@ -328,7 +418,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -514,6 +603,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B7D2-49B5-A24F-D710583116DC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -692,6 +786,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-B7D2-49B5-A24F-D710583116DC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="4"/>
@@ -870,6 +969,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-B7D2-49B5-A24F-D710583116DC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="5"/>
@@ -1048,6 +1152,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-B7D2-49B5-A24F-D710583116DC}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1105,7 +1214,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1188,7 +1296,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -1220,7 +1327,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -1251,7 +1357,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
@@ -1435,6 +1541,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9594-49E9-BED9-82A8C822D89E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
@@ -1545,6 +1656,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-9594-49E9-BED9-82A8C822D89E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="2"/>
@@ -1718,6 +1834,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-9594-49E9-BED9-82A8C822D89E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="3"/>
@@ -1891,6 +2012,11 @@
             </c:numRef>
           </c:yVal>
           <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-9594-49E9-BED9-82A8C822D89E}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1948,7 +2074,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2022,7 +2147,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -2054,7 +2178,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -2085,7 +2208,7 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="1"/>
@@ -2117,7 +2240,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -2319,6 +2441,9 @@
                 </c14:spPr>
               </c14:invertSolidFillFmt>
             </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E46E-4ED8-B5B4-16DF196F6278}"/>
+            </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
@@ -2504,6 +2629,9 @@
                 </c14:spPr>
               </c14:invertSolidFillFmt>
             </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E46E-4ED8-B5B4-16DF196F6278}"/>
+            </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
@@ -2689,6 +2817,9 @@
                 </c14:spPr>
               </c14:invertSolidFillFmt>
             </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E46E-4ED8-B5B4-16DF196F6278}"/>
+            </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
@@ -2874,6 +3005,9 @@
                 </c14:spPr>
               </c14:invertSolidFillFmt>
             </c:ext>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E46E-4ED8-B5B4-16DF196F6278}"/>
+            </c:ext>
           </c:extLst>
         </c:ser>
         <c:ser>
@@ -3040,6 +3174,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-E46E-4ED8-B5B4-16DF196F6278}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="7"/>
@@ -3199,6 +3338,11 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-E46E-4ED8-B5B4-16DF196F6278}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3237,7 +3381,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3320,7 +3463,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -3352,7 +3494,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:txPr>
         <a:bodyPr/>
@@ -3382,6 +3523,986 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metropolis Seeding'!$B$53</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Simple</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metropolis Seeding'!$C$52:$F$52</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Metropolis 8 Threads B[.95,1]</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Metropolis 8 Cooperative Beta = [.95, 1]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Metropolis 8 Cooperative Beta = [.97, .99]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Metropolis 8 Cooperative Beta = [.98, .99]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metropolis Seeding'!$C$53:$F$53</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0674998622215008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88852443075132148</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92518519354128603</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.91839261734219713</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-41C7-4288-83D7-70D2044430C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metropolis Seeding'!$B$54</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Random</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metropolis Seeding'!$C$52:$F$52</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Metropolis 8 Threads B[.95,1]</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Metropolis 8 Cooperative Beta = [.95, 1]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Metropolis 8 Cooperative Beta = [.97, .99]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Metropolis 8 Cooperative Beta = [.98, .99]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metropolis Seeding'!$C$54:$F$54</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.93348856636671751</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.93742602810354914</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92264188989504115</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9304980024255235</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-41C7-4288-83D7-70D2044430C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Metropolis Seeding'!$B$55</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Unassigned neighbor</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Metropolis Seeding'!$C$52:$F$52</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>Metropolis 8 Threads B[.95,1]</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Metropolis 8 Cooperative Beta = [.95, 1]</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Metropolis 8 Cooperative Beta = [.97, .99]</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Metropolis 8 Cooperative Beta = [.98, .99]</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Metropolis Seeding'!$C$55:$F$55</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>0.90004637733104131</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91445019441342956</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.92281041884508264</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.9041305236158178</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-41C7-4288-83D7-70D2044430C2}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="1484407920"/>
+        <c:axId val="1484409584"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="1484407920"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1484409584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1484409584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1484407920"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
@@ -3394,7 +4515,13 @@
     <xdr:ext cx="9448800" cy="5143500"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1" title="Chart"/>
+        <xdr:cNvPr id="2" name="Chart 1" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3411,15 +4538,21 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>59</xdr:row>
-      <xdr:rowOff>66675</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>2105025</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="6915150" cy="4257675"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2" title="Chart"/>
+        <xdr:cNvPr id="3" name="Chart 2" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3444,7 +4577,13 @@
     <xdr:ext cx="14573250" cy="7010400"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3" title="Chart"/>
+        <xdr:cNvPr id="4" name="Chart 3" title="Chart">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -3462,18 +4601,59 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1190625</xdr:colOff>
+      <xdr:row>56</xdr:row>
+      <xdr:rowOff>57149</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>514350</xdr:colOff>
+      <xdr:row>85</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FE0FBC3E-B856-4067-A520-0B9C23DC6F2A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table_1" displayName="Table_1" ref="C3:K25">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="C3:K25">
   <tableColumns count="9">
-    <tableColumn id="1" name="Optimal Coloring"/>
-    <tableColumn id="2" name="Graph Name"/>
-    <tableColumn id="3" name="Vertices"/>
-    <tableColumn id="4" name="Edges"/>
-    <tableColumn id="5" name="Metropolis Coloring"/>
-    <tableColumn id="6" name="Metropolis 8 Threads B[.95,1]"/>
-    <tableColumn id="7" name="Metropolis 8 Cooperative Beta = [.95, 1]"/>
-    <tableColumn id="8" name="Metropolis 8 Cooperative Beta = [.97, .99]"/>
-    <tableColumn id="9" name="Metropolis 8 Cooperative Beta = [.98, .99]"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Optimal Coloring"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Graph Name"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Vertices"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Edges"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Metropolis Coloring"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Metropolis 8 Threads B[.95,1]"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Metropolis 8 Cooperative Beta = [.95, 1]"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Metropolis 8 Cooperative Beta = [.97, .99]"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0000-000009000000}" name="Metropolis 8 Cooperative Beta = [.98, .99]"/>
   </tableColumns>
   <tableStyleInfo name="Sheet1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3676,14 +4856,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A3:AE48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AE25" sqref="AE25"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -7451,4 +8631,2399 @@
     <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34870781-DF0E-4857-B3C0-7B4502F78C19}">
+  <dimension ref="A3:P55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="J74" sqref="J74"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75"/>
+  <cols>
+    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="3" max="3" width="26" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" customWidth="1"/>
+    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.140625" customWidth="1"/>
+    <col min="8" max="8" width="22.42578125" customWidth="1"/>
+    <col min="9" max="9" width="13.5703125" customWidth="1"/>
+    <col min="10" max="10" width="26" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:16" ht="13.5" thickBot="1">
+      <c r="A3" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="K3" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="L3" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="N3" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="O3" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="P3" s="12" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A4" s="7">
+        <v>1</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="7">
+        <v>5</v>
+      </c>
+      <c r="D4" s="8">
+        <v>6</v>
+      </c>
+      <c r="E4" s="8">
+        <v>6</v>
+      </c>
+      <c r="F4" s="8">
+        <v>6</v>
+      </c>
+      <c r="G4" s="8">
+        <v>6</v>
+      </c>
+      <c r="H4" s="8">
+        <v>6</v>
+      </c>
+      <c r="I4" s="10">
+        <v>6</v>
+      </c>
+      <c r="J4" s="10">
+        <v>6</v>
+      </c>
+      <c r="K4" s="10">
+        <v>6</v>
+      </c>
+      <c r="L4" s="10">
+        <v>6</v>
+      </c>
+      <c r="M4" s="11">
+        <v>6</v>
+      </c>
+      <c r="N4" s="11">
+        <v>6</v>
+      </c>
+      <c r="O4" s="11">
+        <v>6</v>
+      </c>
+      <c r="P4" s="11">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A5" s="7">
+        <v>2</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="7">
+        <v>17</v>
+      </c>
+      <c r="D5" s="8">
+        <v>24</v>
+      </c>
+      <c r="E5" s="8">
+        <v>23</v>
+      </c>
+      <c r="F5" s="8">
+        <v>20</v>
+      </c>
+      <c r="G5" s="8">
+        <v>21</v>
+      </c>
+      <c r="H5" s="8">
+        <v>22</v>
+      </c>
+      <c r="I5" s="10">
+        <v>22</v>
+      </c>
+      <c r="J5" s="10">
+        <v>21</v>
+      </c>
+      <c r="K5" s="10">
+        <v>22</v>
+      </c>
+      <c r="L5" s="10">
+        <v>21</v>
+      </c>
+      <c r="M5" s="11">
+        <v>21</v>
+      </c>
+      <c r="N5" s="11">
+        <v>21</v>
+      </c>
+      <c r="O5" s="11">
+        <v>21</v>
+      </c>
+      <c r="P5" s="11">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="16.5" thickBot="1">
+      <c r="A6" s="6">
+        <v>3</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="6">
+        <v>44</v>
+      </c>
+      <c r="D6" s="8">
+        <v>60</v>
+      </c>
+      <c r="E6" s="8">
+        <v>60</v>
+      </c>
+      <c r="F6" s="8">
+        <v>57</v>
+      </c>
+      <c r="G6" s="8">
+        <v>56</v>
+      </c>
+      <c r="H6" s="8">
+        <v>57</v>
+      </c>
+      <c r="I6" s="10">
+        <v>55</v>
+      </c>
+      <c r="J6" s="10">
+        <v>55</v>
+      </c>
+      <c r="K6" s="10">
+        <v>56</v>
+      </c>
+      <c r="L6" s="10">
+        <v>56</v>
+      </c>
+      <c r="M6" s="11">
+        <v>56</v>
+      </c>
+      <c r="N6" s="11">
+        <v>56</v>
+      </c>
+      <c r="O6" s="11">
+        <v>56</v>
+      </c>
+      <c r="P6" s="11">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A7" s="7">
+        <v>4</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="7">
+        <v>8</v>
+      </c>
+      <c r="D7" s="8">
+        <v>11</v>
+      </c>
+      <c r="E7" s="8">
+        <v>11</v>
+      </c>
+      <c r="F7" s="8">
+        <v>10</v>
+      </c>
+      <c r="G7" s="8">
+        <v>10</v>
+      </c>
+      <c r="H7" s="8">
+        <v>10</v>
+      </c>
+      <c r="I7" s="10">
+        <v>10</v>
+      </c>
+      <c r="J7" s="10">
+        <v>10</v>
+      </c>
+      <c r="K7" s="10">
+        <v>10</v>
+      </c>
+      <c r="L7" s="10">
+        <v>10</v>
+      </c>
+      <c r="M7" s="11">
+        <v>10</v>
+      </c>
+      <c r="N7" s="11">
+        <v>10</v>
+      </c>
+      <c r="O7" s="11">
+        <v>10</v>
+      </c>
+      <c r="P7" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A8" s="7">
+        <v>5</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="7">
+        <v>28</v>
+      </c>
+      <c r="D8" s="8">
+        <v>47</v>
+      </c>
+      <c r="E8" s="8">
+        <v>49</v>
+      </c>
+      <c r="F8" s="8">
+        <v>46</v>
+      </c>
+      <c r="G8" s="8">
+        <v>48</v>
+      </c>
+      <c r="H8" s="8">
+        <v>48</v>
+      </c>
+      <c r="I8" s="10">
+        <v>46</v>
+      </c>
+      <c r="J8" s="10">
+        <v>49</v>
+      </c>
+      <c r="K8" s="10">
+        <v>49</v>
+      </c>
+      <c r="L8" s="10">
+        <v>49</v>
+      </c>
+      <c r="M8" s="11">
+        <v>47</v>
+      </c>
+      <c r="N8" s="11">
+        <v>48</v>
+      </c>
+      <c r="O8" s="11">
+        <v>47</v>
+      </c>
+      <c r="P8" s="11">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A9" s="7">
+        <v>6</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="7">
+        <v>72</v>
+      </c>
+      <c r="D9" s="8">
+        <v>135</v>
+      </c>
+      <c r="E9" s="8">
+        <v>131</v>
+      </c>
+      <c r="F9" s="8">
+        <v>128</v>
+      </c>
+      <c r="G9" s="8">
+        <v>131</v>
+      </c>
+      <c r="H9" s="8">
+        <v>133</v>
+      </c>
+      <c r="I9" s="10">
+        <v>137</v>
+      </c>
+      <c r="J9" s="10">
+        <v>129</v>
+      </c>
+      <c r="K9" s="10">
+        <v>130</v>
+      </c>
+      <c r="L9" s="10">
+        <v>134</v>
+      </c>
+      <c r="M9" s="11">
+        <v>130</v>
+      </c>
+      <c r="N9" s="11">
+        <v>132</v>
+      </c>
+      <c r="O9" s="11">
+        <v>131</v>
+      </c>
+      <c r="P9" s="11">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A10" s="7">
+        <v>7</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="7">
+        <v>26</v>
+      </c>
+      <c r="D10" s="8">
+        <v>66</v>
+      </c>
+      <c r="E10" s="8">
+        <v>69</v>
+      </c>
+      <c r="F10" s="8">
+        <v>59</v>
+      </c>
+      <c r="G10" s="8">
+        <v>59</v>
+      </c>
+      <c r="H10" s="8">
+        <v>57</v>
+      </c>
+      <c r="I10" s="10">
+        <v>58</v>
+      </c>
+      <c r="J10" s="10">
+        <v>55</v>
+      </c>
+      <c r="K10" s="10">
+        <v>60</v>
+      </c>
+      <c r="L10" s="10">
+        <v>57</v>
+      </c>
+      <c r="M10" s="11">
+        <v>57</v>
+      </c>
+      <c r="N10" s="11">
+        <v>57</v>
+      </c>
+      <c r="O10" s="11">
+        <v>58</v>
+      </c>
+      <c r="P10" s="11">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A11" s="7">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="7">
+        <v>28</v>
+      </c>
+      <c r="D11" s="8">
+        <v>65</v>
+      </c>
+      <c r="E11" s="8">
+        <v>63</v>
+      </c>
+      <c r="F11" s="8">
+        <v>60</v>
+      </c>
+      <c r="G11" s="8">
+        <v>59</v>
+      </c>
+      <c r="H11" s="8">
+        <v>58</v>
+      </c>
+      <c r="I11" s="10">
+        <v>56</v>
+      </c>
+      <c r="J11" s="10">
+        <v>59</v>
+      </c>
+      <c r="K11" s="10">
+        <v>58</v>
+      </c>
+      <c r="L11" s="10">
+        <v>58</v>
+      </c>
+      <c r="M11" s="11">
+        <v>58</v>
+      </c>
+      <c r="N11" s="11">
+        <v>56</v>
+      </c>
+      <c r="O11" s="11">
+        <v>58</v>
+      </c>
+      <c r="P11" s="11">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A12" s="7">
+        <v>9</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="7">
+        <v>10</v>
+      </c>
+      <c r="D12" s="8">
+        <v>10</v>
+      </c>
+      <c r="E12" s="8">
+        <v>10</v>
+      </c>
+      <c r="F12" s="8">
+        <v>10</v>
+      </c>
+      <c r="G12" s="8">
+        <v>10</v>
+      </c>
+      <c r="H12" s="8">
+        <v>10</v>
+      </c>
+      <c r="I12" s="10">
+        <v>10</v>
+      </c>
+      <c r="J12" s="10">
+        <v>10</v>
+      </c>
+      <c r="K12" s="10">
+        <v>10</v>
+      </c>
+      <c r="L12" s="10">
+        <v>10</v>
+      </c>
+      <c r="M12" s="11">
+        <v>10</v>
+      </c>
+      <c r="N12" s="11">
+        <v>10</v>
+      </c>
+      <c r="O12" s="11">
+        <v>10</v>
+      </c>
+      <c r="P12" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A13" s="7">
+        <v>10</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="7">
+        <v>15</v>
+      </c>
+      <c r="D13" s="8">
+        <v>23</v>
+      </c>
+      <c r="E13" s="8">
+        <v>24</v>
+      </c>
+      <c r="F13" s="8">
+        <v>22</v>
+      </c>
+      <c r="G13" s="8">
+        <v>21</v>
+      </c>
+      <c r="H13" s="8">
+        <v>21</v>
+      </c>
+      <c r="I13" s="10">
+        <v>23</v>
+      </c>
+      <c r="J13" s="10">
+        <v>23</v>
+      </c>
+      <c r="K13" s="10">
+        <v>23</v>
+      </c>
+      <c r="L13" s="10">
+        <v>22</v>
+      </c>
+      <c r="M13" s="11">
+        <v>22</v>
+      </c>
+      <c r="N13" s="11">
+        <v>22</v>
+      </c>
+      <c r="O13" s="11">
+        <v>22</v>
+      </c>
+      <c r="P13" s="11">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A14" s="7">
+        <f t="shared" ref="A14:A24" si="0">A13+1</f>
+        <v>11</v>
+      </c>
+      <c r="B14" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="7">
+        <v>15</v>
+      </c>
+      <c r="D14" s="8">
+        <v>38</v>
+      </c>
+      <c r="E14" s="8">
+        <v>41</v>
+      </c>
+      <c r="F14" s="8">
+        <v>37</v>
+      </c>
+      <c r="G14" s="8">
+        <v>36</v>
+      </c>
+      <c r="H14" s="8">
+        <v>38</v>
+      </c>
+      <c r="I14" s="10">
+        <v>37</v>
+      </c>
+      <c r="J14" s="10">
+        <v>38</v>
+      </c>
+      <c r="K14" s="10">
+        <v>38</v>
+      </c>
+      <c r="L14" s="10">
+        <v>37</v>
+      </c>
+      <c r="M14" s="11">
+        <v>37</v>
+      </c>
+      <c r="N14" s="11">
+        <v>35</v>
+      </c>
+      <c r="O14" s="11">
+        <v>38</v>
+      </c>
+      <c r="P14" s="11">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A15" s="7">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="7">
+        <v>5</v>
+      </c>
+      <c r="D15" s="8">
+        <v>10</v>
+      </c>
+      <c r="E15" s="8">
+        <v>10</v>
+      </c>
+      <c r="F15" s="8">
+        <v>12</v>
+      </c>
+      <c r="G15" s="8">
+        <v>12</v>
+      </c>
+      <c r="H15" s="8">
+        <v>10</v>
+      </c>
+      <c r="I15" s="10">
+        <v>11</v>
+      </c>
+      <c r="J15" s="10">
+        <v>12</v>
+      </c>
+      <c r="K15" s="10">
+        <v>11</v>
+      </c>
+      <c r="L15" s="10">
+        <v>12</v>
+      </c>
+      <c r="M15" s="11">
+        <v>12</v>
+      </c>
+      <c r="N15" s="11">
+        <v>11</v>
+      </c>
+      <c r="O15" s="11">
+        <v>11</v>
+      </c>
+      <c r="P15" s="11">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A16" s="7">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="7">
+        <v>5</v>
+      </c>
+      <c r="D16" s="8">
+        <v>13</v>
+      </c>
+      <c r="E16" s="8">
+        <v>15</v>
+      </c>
+      <c r="F16" s="8">
+        <v>10</v>
+      </c>
+      <c r="G16" s="8">
+        <v>12</v>
+      </c>
+      <c r="H16" s="8">
+        <v>12</v>
+      </c>
+      <c r="I16" s="10">
+        <v>12</v>
+      </c>
+      <c r="J16" s="10">
+        <v>12</v>
+      </c>
+      <c r="K16" s="10">
+        <v>11</v>
+      </c>
+      <c r="L16" s="10">
+        <v>11</v>
+      </c>
+      <c r="M16" s="11">
+        <v>12</v>
+      </c>
+      <c r="N16" s="11">
+        <v>12</v>
+      </c>
+      <c r="O16" s="11">
+        <v>12</v>
+      </c>
+      <c r="P16" s="11">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A17" s="7">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="7">
+        <v>20</v>
+      </c>
+      <c r="D17" s="8">
+        <v>33</v>
+      </c>
+      <c r="E17" s="8">
+        <v>29</v>
+      </c>
+      <c r="F17" s="8">
+        <v>29</v>
+      </c>
+      <c r="G17" s="8">
+        <v>28</v>
+      </c>
+      <c r="H17" s="8">
+        <v>27</v>
+      </c>
+      <c r="I17" s="10">
+        <v>29</v>
+      </c>
+      <c r="J17" s="10">
+        <v>30</v>
+      </c>
+      <c r="K17" s="10">
+        <v>28</v>
+      </c>
+      <c r="L17" s="10">
+        <v>31</v>
+      </c>
+      <c r="M17" s="11">
+        <v>28</v>
+      </c>
+      <c r="N17" s="11">
+        <v>29</v>
+      </c>
+      <c r="O17" s="11">
+        <v>28</v>
+      </c>
+      <c r="P17" s="11">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A18" s="7">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B18" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="7">
+        <v>5</v>
+      </c>
+      <c r="D18" s="8">
+        <v>5</v>
+      </c>
+      <c r="E18" s="8">
+        <v>5</v>
+      </c>
+      <c r="F18" s="8">
+        <v>5</v>
+      </c>
+      <c r="G18" s="8">
+        <v>5</v>
+      </c>
+      <c r="H18" s="8">
+        <v>5</v>
+      </c>
+      <c r="I18" s="10">
+        <v>5</v>
+      </c>
+      <c r="J18" s="10">
+        <v>5</v>
+      </c>
+      <c r="K18" s="10">
+        <v>5</v>
+      </c>
+      <c r="L18" s="10">
+        <v>5</v>
+      </c>
+      <c r="M18" s="11">
+        <v>5</v>
+      </c>
+      <c r="N18" s="11">
+        <v>5</v>
+      </c>
+      <c r="O18" s="11">
+        <v>5</v>
+      </c>
+      <c r="P18" s="11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A19" s="7">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="7">
+        <v>36</v>
+      </c>
+      <c r="D19" s="8">
+        <v>44</v>
+      </c>
+      <c r="E19" s="8">
+        <v>46</v>
+      </c>
+      <c r="F19" s="8">
+        <v>41</v>
+      </c>
+      <c r="G19" s="8">
+        <v>41</v>
+      </c>
+      <c r="H19" s="8">
+        <v>42</v>
+      </c>
+      <c r="I19" s="10">
+        <v>42</v>
+      </c>
+      <c r="J19" s="10">
+        <v>42</v>
+      </c>
+      <c r="K19" s="10">
+        <v>42</v>
+      </c>
+      <c r="L19" s="10">
+        <v>42</v>
+      </c>
+      <c r="M19" s="11">
+        <v>42</v>
+      </c>
+      <c r="N19" s="11">
+        <v>42</v>
+      </c>
+      <c r="O19" s="11">
+        <v>43</v>
+      </c>
+      <c r="P19" s="11">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A20" s="7">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="7">
+        <v>8</v>
+      </c>
+      <c r="D20" s="8">
+        <v>8</v>
+      </c>
+      <c r="E20" s="8">
+        <v>8</v>
+      </c>
+      <c r="F20" s="8">
+        <v>8</v>
+      </c>
+      <c r="G20" s="8">
+        <v>8</v>
+      </c>
+      <c r="H20" s="8">
+        <v>8</v>
+      </c>
+      <c r="I20" s="10">
+        <v>8</v>
+      </c>
+      <c r="J20" s="10">
+        <v>8</v>
+      </c>
+      <c r="K20" s="10">
+        <v>8</v>
+      </c>
+      <c r="L20" s="10">
+        <v>8</v>
+      </c>
+      <c r="M20" s="11">
+        <v>8</v>
+      </c>
+      <c r="N20" s="11">
+        <v>8</v>
+      </c>
+      <c r="O20" s="11">
+        <v>8</v>
+      </c>
+      <c r="P20" s="11">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A21" s="7">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="7">
+        <v>64</v>
+      </c>
+      <c r="D21" s="8">
+        <v>182</v>
+      </c>
+      <c r="E21" s="8">
+        <v>175</v>
+      </c>
+      <c r="F21" s="8">
+        <v>168</v>
+      </c>
+      <c r="G21" s="8">
+        <v>171</v>
+      </c>
+      <c r="H21" s="8">
+        <v>176</v>
+      </c>
+      <c r="I21" s="10">
+        <v>172</v>
+      </c>
+      <c r="J21" s="10">
+        <v>173</v>
+      </c>
+      <c r="K21" s="10">
+        <v>169</v>
+      </c>
+      <c r="L21" s="10">
+        <v>171</v>
+      </c>
+      <c r="M21" s="11">
+        <v>167</v>
+      </c>
+      <c r="N21" s="11">
+        <v>173</v>
+      </c>
+      <c r="O21" s="11">
+        <v>169</v>
+      </c>
+      <c r="P21" s="11">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A22" s="7">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B22" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C22" s="7">
+        <v>28</v>
+      </c>
+      <c r="D22" s="8">
+        <v>92</v>
+      </c>
+      <c r="E22" s="8">
+        <v>94</v>
+      </c>
+      <c r="F22" s="8">
+        <v>88</v>
+      </c>
+      <c r="G22" s="8">
+        <v>89</v>
+      </c>
+      <c r="H22" s="8">
+        <v>87</v>
+      </c>
+      <c r="I22" s="10">
+        <v>88</v>
+      </c>
+      <c r="J22" s="10">
+        <v>89</v>
+      </c>
+      <c r="K22" s="10">
+        <v>87</v>
+      </c>
+      <c r="L22" s="10">
+        <v>86</v>
+      </c>
+      <c r="M22" s="11">
+        <v>86</v>
+      </c>
+      <c r="N22" s="11">
+        <v>88</v>
+      </c>
+      <c r="O22" s="11">
+        <v>86</v>
+      </c>
+      <c r="P22" s="11">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A23" s="7">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="7">
+        <v>14</v>
+      </c>
+      <c r="D23" s="8">
+        <v>54</v>
+      </c>
+      <c r="E23" s="8">
+        <v>55</v>
+      </c>
+      <c r="F23" s="8">
+        <v>45</v>
+      </c>
+      <c r="G23" s="8">
+        <v>46</v>
+      </c>
+      <c r="H23" s="8">
+        <v>44</v>
+      </c>
+      <c r="I23" s="10">
+        <v>48</v>
+      </c>
+      <c r="J23" s="10">
+        <v>46</v>
+      </c>
+      <c r="K23" s="10">
+        <v>47</v>
+      </c>
+      <c r="L23" s="10">
+        <v>45</v>
+      </c>
+      <c r="M23" s="11">
+        <v>45</v>
+      </c>
+      <c r="N23" s="11">
+        <v>47</v>
+      </c>
+      <c r="O23" s="11">
+        <v>48</v>
+      </c>
+      <c r="P23" s="11">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" ht="15.75" thickBot="1">
+      <c r="A24" s="7">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="7">
+        <v>14</v>
+      </c>
+      <c r="D24" s="8">
+        <v>62</v>
+      </c>
+      <c r="E24" s="8">
+        <v>64</v>
+      </c>
+      <c r="F24" s="8">
+        <v>56</v>
+      </c>
+      <c r="G24" s="8">
+        <v>60</v>
+      </c>
+      <c r="H24" s="8">
+        <v>64</v>
+      </c>
+      <c r="I24" s="10">
+        <v>61</v>
+      </c>
+      <c r="J24" s="10">
+        <v>60</v>
+      </c>
+      <c r="K24" s="10">
+        <v>60</v>
+      </c>
+      <c r="L24" s="10">
+        <v>63</v>
+      </c>
+      <c r="M24" s="11">
+        <v>56</v>
+      </c>
+      <c r="N24" s="11">
+        <v>60</v>
+      </c>
+      <c r="O24" s="11">
+        <v>60</v>
+      </c>
+      <c r="P24" s="11">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16">
+      <c r="D27" s="9">
+        <f>(D4-$C4)/$C4</f>
+        <v>0.2</v>
+      </c>
+      <c r="E27" s="9">
+        <f t="shared" ref="E27:P27" si="1">(E4-$C4)/$C4</f>
+        <v>0.2</v>
+      </c>
+      <c r="F27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="G27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="H27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="I27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="J27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="K27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="L27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="M27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="N27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="O27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="P27" s="9">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16">
+      <c r="D28" s="9">
+        <f t="shared" ref="D28:P47" si="2">(D5-$C5)/$C5</f>
+        <v>0.41176470588235292</v>
+      </c>
+      <c r="E28" s="9">
+        <f t="shared" si="2"/>
+        <v>0.35294117647058826</v>
+      </c>
+      <c r="F28" s="9">
+        <f t="shared" si="2"/>
+        <v>0.17647058823529413</v>
+      </c>
+      <c r="G28" s="9">
+        <f t="shared" si="2"/>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="H28" s="9">
+        <f t="shared" si="2"/>
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="I28" s="9">
+        <f t="shared" si="2"/>
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="J28" s="9">
+        <f t="shared" si="2"/>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="K28" s="9">
+        <f t="shared" si="2"/>
+        <v>0.29411764705882354</v>
+      </c>
+      <c r="L28" s="9">
+        <f t="shared" si="2"/>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="M28" s="9">
+        <f t="shared" si="2"/>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="N28" s="9">
+        <f t="shared" si="2"/>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="O28" s="9">
+        <f t="shared" si="2"/>
+        <v>0.23529411764705882</v>
+      </c>
+      <c r="P28" s="9">
+        <f t="shared" si="2"/>
+        <v>0.29411764705882354</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16">
+      <c r="D29" s="9">
+        <f t="shared" si="2"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="E29" s="9">
+        <f t="shared" si="2"/>
+        <v>0.36363636363636365</v>
+      </c>
+      <c r="F29" s="9">
+        <f t="shared" si="2"/>
+        <v>0.29545454545454547</v>
+      </c>
+      <c r="G29" s="9">
+        <f t="shared" si="2"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="H29" s="9">
+        <f t="shared" si="2"/>
+        <v>0.29545454545454547</v>
+      </c>
+      <c r="I29" s="9">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="J29" s="9">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="K29" s="9">
+        <f t="shared" si="2"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="L29" s="9">
+        <f t="shared" si="2"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="M29" s="9">
+        <f t="shared" si="2"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="N29" s="9">
+        <f t="shared" si="2"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="O29" s="9">
+        <f t="shared" si="2"/>
+        <v>0.27272727272727271</v>
+      </c>
+      <c r="P29" s="9">
+        <f t="shared" si="2"/>
+        <v>0.29545454545454547</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16">
+      <c r="D30" s="9">
+        <f t="shared" si="2"/>
+        <v>0.375</v>
+      </c>
+      <c r="E30" s="9">
+        <f t="shared" si="2"/>
+        <v>0.375</v>
+      </c>
+      <c r="F30" s="9">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="G30" s="9">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="H30" s="9">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="I30" s="9">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="J30" s="9">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="K30" s="9">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="L30" s="9">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="M30" s="9">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="N30" s="9">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="O30" s="9">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="P30" s="9">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16">
+      <c r="D31" s="9">
+        <f t="shared" si="2"/>
+        <v>0.6785714285714286</v>
+      </c>
+      <c r="E31" s="9">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="F31" s="9">
+        <f t="shared" si="2"/>
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="G31" s="9">
+        <f t="shared" si="2"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="H31" s="9">
+        <f t="shared" si="2"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="I31" s="9">
+        <f t="shared" si="2"/>
+        <v>0.6428571428571429</v>
+      </c>
+      <c r="J31" s="9">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="K31" s="9">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="L31" s="9">
+        <f t="shared" si="2"/>
+        <v>0.75</v>
+      </c>
+      <c r="M31" s="9">
+        <f t="shared" si="2"/>
+        <v>0.6785714285714286</v>
+      </c>
+      <c r="N31" s="9">
+        <f t="shared" si="2"/>
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="O31" s="9">
+        <f t="shared" si="2"/>
+        <v>0.6785714285714286</v>
+      </c>
+      <c r="P31" s="9">
+        <f t="shared" si="2"/>
+        <v>0.7142857142857143</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16">
+      <c r="D32" s="9">
+        <f t="shared" si="2"/>
+        <v>0.875</v>
+      </c>
+      <c r="E32" s="9">
+        <f t="shared" si="2"/>
+        <v>0.81944444444444442</v>
+      </c>
+      <c r="F32" s="9">
+        <f t="shared" si="2"/>
+        <v>0.77777777777777779</v>
+      </c>
+      <c r="G32" s="9">
+        <f t="shared" si="2"/>
+        <v>0.81944444444444442</v>
+      </c>
+      <c r="H32" s="9">
+        <f t="shared" si="2"/>
+        <v>0.84722222222222221</v>
+      </c>
+      <c r="I32" s="9">
+        <f t="shared" si="2"/>
+        <v>0.90277777777777779</v>
+      </c>
+      <c r="J32" s="9">
+        <f t="shared" si="2"/>
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="K32" s="9">
+        <f t="shared" si="2"/>
+        <v>0.80555555555555558</v>
+      </c>
+      <c r="L32" s="9">
+        <f t="shared" si="2"/>
+        <v>0.86111111111111116</v>
+      </c>
+      <c r="M32" s="9">
+        <f t="shared" si="2"/>
+        <v>0.80555555555555558</v>
+      </c>
+      <c r="N32" s="9">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333337</v>
+      </c>
+      <c r="O32" s="9">
+        <f t="shared" si="2"/>
+        <v>0.81944444444444442</v>
+      </c>
+      <c r="P32" s="9">
+        <f t="shared" si="2"/>
+        <v>0.79166666666666663</v>
+      </c>
+    </row>
+    <row r="33" spans="4:16">
+      <c r="D33" s="9">
+        <f t="shared" si="2"/>
+        <v>1.5384615384615385</v>
+      </c>
+      <c r="E33" s="9">
+        <f t="shared" si="2"/>
+        <v>1.6538461538461537</v>
+      </c>
+      <c r="F33" s="9">
+        <f t="shared" si="2"/>
+        <v>1.2692307692307692</v>
+      </c>
+      <c r="G33" s="9">
+        <f t="shared" si="2"/>
+        <v>1.2692307692307692</v>
+      </c>
+      <c r="H33" s="9">
+        <f t="shared" si="2"/>
+        <v>1.1923076923076923</v>
+      </c>
+      <c r="I33" s="9">
+        <f t="shared" si="2"/>
+        <v>1.2307692307692308</v>
+      </c>
+      <c r="J33" s="9">
+        <f t="shared" si="2"/>
+        <v>1.1153846153846154</v>
+      </c>
+      <c r="K33" s="9">
+        <f t="shared" si="2"/>
+        <v>1.3076923076923077</v>
+      </c>
+      <c r="L33" s="9">
+        <f t="shared" si="2"/>
+        <v>1.1923076923076923</v>
+      </c>
+      <c r="M33" s="9">
+        <f t="shared" si="2"/>
+        <v>1.1923076923076923</v>
+      </c>
+      <c r="N33" s="9">
+        <f t="shared" si="2"/>
+        <v>1.1923076923076923</v>
+      </c>
+      <c r="O33" s="9">
+        <f t="shared" si="2"/>
+        <v>1.2307692307692308</v>
+      </c>
+      <c r="P33" s="9">
+        <f t="shared" si="2"/>
+        <v>1.1923076923076923</v>
+      </c>
+    </row>
+    <row r="34" spans="4:16">
+      <c r="D34" s="9">
+        <f t="shared" si="2"/>
+        <v>1.3214285714285714</v>
+      </c>
+      <c r="E34" s="9">
+        <f t="shared" si="2"/>
+        <v>1.25</v>
+      </c>
+      <c r="F34" s="9">
+        <f t="shared" si="2"/>
+        <v>1.1428571428571428</v>
+      </c>
+      <c r="G34" s="9">
+        <f t="shared" si="2"/>
+        <v>1.1071428571428572</v>
+      </c>
+      <c r="H34" s="9">
+        <f t="shared" si="2"/>
+        <v>1.0714285714285714</v>
+      </c>
+      <c r="I34" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="J34" s="9">
+        <f t="shared" si="2"/>
+        <v>1.1071428571428572</v>
+      </c>
+      <c r="K34" s="9">
+        <f t="shared" si="2"/>
+        <v>1.0714285714285714</v>
+      </c>
+      <c r="L34" s="9">
+        <f t="shared" si="2"/>
+        <v>1.0714285714285714</v>
+      </c>
+      <c r="M34" s="9">
+        <f t="shared" si="2"/>
+        <v>1.0714285714285714</v>
+      </c>
+      <c r="N34" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="O34" s="9">
+        <f t="shared" si="2"/>
+        <v>1.0714285714285714</v>
+      </c>
+      <c r="P34" s="9">
+        <f t="shared" si="2"/>
+        <v>1.1428571428571428</v>
+      </c>
+    </row>
+    <row r="35" spans="4:16">
+      <c r="D35" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E35" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F35" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G35" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H35" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I35" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J35" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K35" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L35" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M35" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N35" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O35" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P35" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="4:16">
+      <c r="D36" s="9">
+        <f t="shared" si="2"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="E36" s="9">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+      <c r="F36" s="9">
+        <f t="shared" si="2"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="G36" s="9">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="H36" s="9">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="I36" s="9">
+        <f t="shared" si="2"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="J36" s="9">
+        <f t="shared" si="2"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="K36" s="9">
+        <f t="shared" si="2"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="L36" s="9">
+        <f t="shared" si="2"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="M36" s="9">
+        <f t="shared" si="2"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="N36" s="9">
+        <f t="shared" si="2"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="O36" s="9">
+        <f t="shared" si="2"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="P36" s="9">
+        <f t="shared" si="2"/>
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="37" spans="4:16">
+      <c r="D37" s="9">
+        <f t="shared" si="2"/>
+        <v>1.5333333333333334</v>
+      </c>
+      <c r="E37" s="9">
+        <f t="shared" si="2"/>
+        <v>1.7333333333333334</v>
+      </c>
+      <c r="F37" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4666666666666666</v>
+      </c>
+      <c r="G37" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="H37" s="9">
+        <f t="shared" si="2"/>
+        <v>1.5333333333333334</v>
+      </c>
+      <c r="I37" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4666666666666666</v>
+      </c>
+      <c r="J37" s="9">
+        <f t="shared" si="2"/>
+        <v>1.5333333333333334</v>
+      </c>
+      <c r="K37" s="9">
+        <f t="shared" si="2"/>
+        <v>1.5333333333333334</v>
+      </c>
+      <c r="L37" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4666666666666666</v>
+      </c>
+      <c r="M37" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4666666666666666</v>
+      </c>
+      <c r="N37" s="9">
+        <f t="shared" si="2"/>
+        <v>1.3333333333333333</v>
+      </c>
+      <c r="O37" s="9">
+        <f t="shared" si="2"/>
+        <v>1.5333333333333334</v>
+      </c>
+      <c r="P37" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4666666666666666</v>
+      </c>
+    </row>
+    <row r="38" spans="4:16">
+      <c r="D38" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="E38" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="F38" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="G38" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="H38" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="I38" s="9">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+      <c r="J38" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="K38" s="9">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+      <c r="L38" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="M38" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="N38" s="9">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+      <c r="O38" s="9">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+      <c r="P38" s="9">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="39" spans="4:16">
+      <c r="D39" s="9">
+        <f t="shared" si="2"/>
+        <v>1.6</v>
+      </c>
+      <c r="E39" s="9">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="F39" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="G39" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="H39" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="I39" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="J39" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="K39" s="9">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+      <c r="L39" s="9">
+        <f t="shared" si="2"/>
+        <v>1.2</v>
+      </c>
+      <c r="M39" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="N39" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="O39" s="9">
+        <f t="shared" si="2"/>
+        <v>1.4</v>
+      </c>
+      <c r="P39" s="9">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="4:16">
+      <c r="D40" s="9">
+        <f t="shared" si="2"/>
+        <v>0.65</v>
+      </c>
+      <c r="E40" s="9">
+        <f t="shared" si="2"/>
+        <v>0.45</v>
+      </c>
+      <c r="F40" s="9">
+        <f t="shared" si="2"/>
+        <v>0.45</v>
+      </c>
+      <c r="G40" s="9">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="H40" s="9">
+        <f t="shared" si="2"/>
+        <v>0.35</v>
+      </c>
+      <c r="I40" s="9">
+        <f t="shared" si="2"/>
+        <v>0.45</v>
+      </c>
+      <c r="J40" s="9">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="K40" s="9">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="L40" s="9">
+        <f t="shared" si="2"/>
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="M40" s="9">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="N40" s="9">
+        <f t="shared" si="2"/>
+        <v>0.45</v>
+      </c>
+      <c r="O40" s="9">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+      <c r="P40" s="9">
+        <f t="shared" si="2"/>
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="41" spans="4:16">
+      <c r="D41" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E41" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F41" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G41" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H41" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I41" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J41" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K41" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L41" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M41" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N41" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O41" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P41" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="4:16">
+      <c r="D42" s="9">
+        <f t="shared" si="2"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="E42" s="9">
+        <f t="shared" si="2"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="F42" s="9">
+        <f t="shared" si="2"/>
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="G42" s="9">
+        <f t="shared" si="2"/>
+        <v>0.1388888888888889</v>
+      </c>
+      <c r="H42" s="9">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="I42" s="9">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="J42" s="9">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="K42" s="9">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="L42" s="9">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="M42" s="9">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="N42" s="9">
+        <f t="shared" si="2"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="O42" s="9">
+        <f t="shared" si="2"/>
+        <v>0.19444444444444445</v>
+      </c>
+      <c r="P42" s="9">
+        <f t="shared" si="2"/>
+        <v>0.19444444444444445</v>
+      </c>
+    </row>
+    <row r="43" spans="4:16">
+      <c r="D43" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E43" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F43" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G43" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H43" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I43" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J43" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="K43" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L43" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M43" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N43" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O43" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P43" s="9">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="4:16">
+      <c r="D44" s="9">
+        <f t="shared" si="2"/>
+        <v>1.84375</v>
+      </c>
+      <c r="E44" s="9">
+        <f t="shared" si="2"/>
+        <v>1.734375</v>
+      </c>
+      <c r="F44" s="9">
+        <f t="shared" si="2"/>
+        <v>1.625</v>
+      </c>
+      <c r="G44" s="9">
+        <f t="shared" si="2"/>
+        <v>1.671875</v>
+      </c>
+      <c r="H44" s="9">
+        <f t="shared" si="2"/>
+        <v>1.75</v>
+      </c>
+      <c r="I44" s="9">
+        <f t="shared" si="2"/>
+        <v>1.6875</v>
+      </c>
+      <c r="J44" s="9">
+        <f t="shared" si="2"/>
+        <v>1.703125</v>
+      </c>
+      <c r="K44" s="9">
+        <f t="shared" si="2"/>
+        <v>1.640625</v>
+      </c>
+      <c r="L44" s="9">
+        <f t="shared" si="2"/>
+        <v>1.671875</v>
+      </c>
+      <c r="M44" s="9">
+        <f t="shared" si="2"/>
+        <v>1.609375</v>
+      </c>
+      <c r="N44" s="9">
+        <f t="shared" si="2"/>
+        <v>1.703125</v>
+      </c>
+      <c r="O44" s="9">
+        <f t="shared" si="2"/>
+        <v>1.640625</v>
+      </c>
+      <c r="P44" s="9">
+        <f t="shared" si="2"/>
+        <v>1.71875</v>
+      </c>
+    </row>
+    <row r="45" spans="4:16">
+      <c r="D45" s="9">
+        <f t="shared" si="2"/>
+        <v>2.2857142857142856</v>
+      </c>
+      <c r="E45" s="9">
+        <f t="shared" si="2"/>
+        <v>2.3571428571428572</v>
+      </c>
+      <c r="F45" s="9">
+        <f t="shared" si="2"/>
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="G45" s="9">
+        <f t="shared" si="2"/>
+        <v>2.1785714285714284</v>
+      </c>
+      <c r="H45" s="9">
+        <f t="shared" si="2"/>
+        <v>2.1071428571428572</v>
+      </c>
+      <c r="I45" s="9">
+        <f t="shared" si="2"/>
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="J45" s="9">
+        <f t="shared" si="2"/>
+        <v>2.1785714285714284</v>
+      </c>
+      <c r="K45" s="9">
+        <f t="shared" si="2"/>
+        <v>2.1071428571428572</v>
+      </c>
+      <c r="L45" s="9">
+        <f t="shared" si="2"/>
+        <v>2.0714285714285716</v>
+      </c>
+      <c r="M45" s="9">
+        <f t="shared" si="2"/>
+        <v>2.0714285714285716</v>
+      </c>
+      <c r="N45" s="9">
+        <f t="shared" si="2"/>
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="O45" s="9">
+        <f t="shared" si="2"/>
+        <v>2.0714285714285716</v>
+      </c>
+      <c r="P45" s="9">
+        <f t="shared" si="2"/>
+        <v>2.1428571428571428</v>
+      </c>
+    </row>
+    <row r="46" spans="4:16">
+      <c r="D46" s="9">
+        <f t="shared" si="2"/>
+        <v>2.8571428571428572</v>
+      </c>
+      <c r="E46" s="9">
+        <f t="shared" si="2"/>
+        <v>2.9285714285714284</v>
+      </c>
+      <c r="F46" s="9">
+        <f t="shared" si="2"/>
+        <v>2.2142857142857144</v>
+      </c>
+      <c r="G46" s="9">
+        <f t="shared" si="2"/>
+        <v>2.2857142857142856</v>
+      </c>
+      <c r="H46" s="9">
+        <f t="shared" si="2"/>
+        <v>2.1428571428571428</v>
+      </c>
+      <c r="I46" s="9">
+        <f t="shared" si="2"/>
+        <v>2.4285714285714284</v>
+      </c>
+      <c r="J46" s="9">
+        <f t="shared" si="2"/>
+        <v>2.2857142857142856</v>
+      </c>
+      <c r="K46" s="9">
+        <f t="shared" si="2"/>
+        <v>2.3571428571428572</v>
+      </c>
+      <c r="L46" s="9">
+        <f t="shared" si="2"/>
+        <v>2.2142857142857144</v>
+      </c>
+      <c r="M46" s="9">
+        <f t="shared" si="2"/>
+        <v>2.2142857142857144</v>
+      </c>
+      <c r="N46" s="9">
+        <f t="shared" si="2"/>
+        <v>2.3571428571428572</v>
+      </c>
+      <c r="O46" s="9">
+        <f t="shared" si="2"/>
+        <v>2.4285714285714284</v>
+      </c>
+      <c r="P46" s="9">
+        <f t="shared" si="2"/>
+        <v>2.2857142857142856</v>
+      </c>
+    </row>
+    <row r="47" spans="4:16">
+      <c r="D47" s="9">
+        <f t="shared" si="2"/>
+        <v>3.4285714285714284</v>
+      </c>
+      <c r="E47" s="9">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="F47" s="9">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="G47" s="9">
+        <f t="shared" si="2"/>
+        <v>3.2857142857142856</v>
+      </c>
+      <c r="H47" s="9">
+        <f t="shared" si="2"/>
+        <v>3.5714285714285716</v>
+      </c>
+      <c r="I47" s="9">
+        <f t="shared" si="2"/>
+        <v>3.3571428571428572</v>
+      </c>
+      <c r="J47" s="9">
+        <f t="shared" si="2"/>
+        <v>3.2857142857142856</v>
+      </c>
+      <c r="K47" s="9">
+        <f t="shared" si="2"/>
+        <v>3.2857142857142856</v>
+      </c>
+      <c r="L47" s="9">
+        <f t="shared" ref="L47:P47" si="3">(L24-$C24)/$C24</f>
+        <v>3.5</v>
+      </c>
+      <c r="M47" s="9">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+      <c r="N47" s="9">
+        <f t="shared" si="3"/>
+        <v>3.2857142857142856</v>
+      </c>
+      <c r="O47" s="9">
+        <f t="shared" si="3"/>
+        <v>3.2857142857142856</v>
+      </c>
+      <c r="P47" s="9">
+        <f t="shared" si="3"/>
+        <v>3.2142857142857144</v>
+      </c>
+    </row>
+    <row r="48" spans="4:16">
+      <c r="D48" s="9">
+        <f t="shared" ref="D48:P48" si="4">AVERAGE(D27:D47)</f>
+        <v>1.0341871461094148</v>
+      </c>
+      <c r="E48" s="9">
+        <f t="shared" si="4"/>
+        <v>1.0674998622215008</v>
+      </c>
+      <c r="F48" s="9">
+        <f t="shared" si="4"/>
+        <v>0.88852443075132148</v>
+      </c>
+      <c r="G48" s="9">
+        <f t="shared" si="4"/>
+        <v>0.92518519354128603</v>
+      </c>
+      <c r="H48" s="9">
+        <f t="shared" si="4"/>
+        <v>0.91839261734219713</v>
+      </c>
+      <c r="I48" s="9">
+        <f t="shared" si="4"/>
+        <v>0.93348856636671751</v>
+      </c>
+      <c r="J48" s="9">
+        <f t="shared" si="4"/>
+        <v>0.93742602810354914</v>
+      </c>
+      <c r="K48" s="9">
+        <f t="shared" si="4"/>
+        <v>0.92264188989504115</v>
+      </c>
+      <c r="L48" s="9">
+        <f t="shared" si="4"/>
+        <v>0.9304980024255235</v>
+      </c>
+      <c r="M48" s="9">
+        <f t="shared" si="4"/>
+        <v>0.90004637733104131</v>
+      </c>
+      <c r="N48" s="9">
+        <f t="shared" si="4"/>
+        <v>0.91445019441342956</v>
+      </c>
+      <c r="O48" s="9">
+        <f t="shared" si="4"/>
+        <v>0.92281041884508264</v>
+      </c>
+      <c r="P48" s="9">
+        <f t="shared" si="4"/>
+        <v>0.9041305236158178</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6">
+      <c r="B52" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C52" t="s">
+        <v>7</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="F52" s="8" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6">
+      <c r="B53" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="C53">
+        <v>1.0674998622215008</v>
+      </c>
+      <c r="D53">
+        <v>0.88852443075132148</v>
+      </c>
+      <c r="E53">
+        <v>0.92518519354128603</v>
+      </c>
+      <c r="F53">
+        <v>0.91839261734219713</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6">
+      <c r="B54" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C54" s="9">
+        <v>0.93348856636671751</v>
+      </c>
+      <c r="D54" s="9">
+        <v>0.93742602810354914</v>
+      </c>
+      <c r="E54" s="9">
+        <v>0.92264188989504115</v>
+      </c>
+      <c r="F54" s="9">
+        <v>0.9304980024255235</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="C55" s="9">
+        <v>0.90004637733104131</v>
+      </c>
+      <c r="D55" s="9">
+        <v>0.91445019441342956</v>
+      </c>
+      <c r="E55" s="9">
+        <v>0.92281041884508264</v>
+      </c>
+      <c r="F55" s="9">
+        <v>0.9041305236158178</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>